<commit_message>
Modified BOM format and added new column for board name to make sorting parts easier.
</commit_message>
<xml_diff>
--- a/compact_LTM4607_PCB/doc/carrier/carrier_board_simplified.xlsx
+++ b/compact_LTM4607_PCB/doc/carrier/carrier_board_simplified.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b59mi\Documents\Business\ARVP\compact_LTM4607_PCB\doc\carrier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b59mi\Documents\Business\ARVP\au_hardware\compact_LTM4607_PCB\doc\carrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -300,10 +300,10 @@
     <t>http://www.on-shore.com/wp-content/uploads/2015/09/OSTT7XX0150.pdf</t>
   </si>
   <si>
-    <t>Received?</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>CARRIER</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -754,6 +754,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -800,24 +815,27 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1143,7 +1161,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,40 +1173,41 @@
     <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1199,65 +1218,66 @@
       <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="5">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="5">
         <f>A2*I2</f>
         <v>0.20399999999999999</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="9">
         <v>0.32</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="9">
         <f t="shared" ref="J3:J18" si="0">A3*I3</f>
         <v>0.96</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1268,32 +1288,33 @@
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="1" t="str">
+      <c r="D4" s="10" t="str">
         <f>"3557-10"</f>
         <v>3557-10</v>
       </c>
-      <c r="E4" s="1" t="str">
+      <c r="E4" s="10" t="str">
         <f>"3557-10"</f>
         <v>3557-10</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="F4" s="4"/>
+      <c r="G4" s="10" t="str">
         <f>"3557-10"</f>
         <v>3557-10</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="5">
         <v>1.43</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="5">
         <f t="shared" si="0"/>
         <v>1.43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1304,29 +1325,30 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="11">
         <v>0.52</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1337,95 +1359,96 @@
       <c r="B6">
         <v>0.5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="11">
         <v>0.78</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="5">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="14">
         <v>0.4</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="9">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>0.63</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="9">
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1436,29 +1459,30 @@
       <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="11">
         <v>2.29</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="5">
         <f t="shared" si="0"/>
         <v>6.87</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1469,32 +1493,32 @@
       <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="11">
         <v>3.9E-2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="5">
         <f t="shared" si="0"/>
         <v>0.23399999999999999</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1505,32 +1529,32 @@
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="11">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="5">
         <f t="shared" si="0"/>
         <v>0.14400000000000002</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1541,32 +1565,32 @@
       <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="11">
         <v>1.47</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
         <v>4.41</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1577,29 +1601,30 @@
       <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="11">
         <v>0.81</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="5">
         <f t="shared" si="0"/>
         <v>2.4300000000000002</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1607,65 +1632,66 @@
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="11">
         <v>4.51</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="5">
         <f t="shared" si="0"/>
         <v>13.53</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="9">
         <v>2.13</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="9">
         <f t="shared" si="0"/>
         <v>2.13</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1673,29 +1699,30 @@
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="11">
         <v>4.96</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="5">
         <f t="shared" si="0"/>
         <v>14.879999999999999</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1703,67 +1730,70 @@
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="11">
         <v>19.22</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="5">
         <f t="shared" si="0"/>
         <v>57.66</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>2.1800000000000002</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="9">
         <f t="shared" si="0"/>
         <v>2.1800000000000002</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I20" s="3" t="s">
+      <c r="F20" s="15"/>
+      <c r="I20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <f>SUM(J2:J18)</f>
         <v>109.39200000000001</v>
       </c>

</xml_diff>